<commit_message>
Added the code of some graphs
</commit_message>
<xml_diff>
--- a/Harmonization_table_varnames.xlsx
+++ b/Harmonization_table_varnames.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofnottm-my.sharepoint.com/personal/geertje_veeken2_nottingham_ac_uk/Documents/Data analysis/Placement/OPN/gender_covid_opn/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgxgv\OneDrive - The University of Nottingham\Data analysis\Placement\OPN\gender_covid_opn\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7435" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7435" uniqueCount="309">
   <si>
     <t>var.name</t>
   </si>
@@ -937,9 +937,6 @@
   </si>
   <si>
     <t>y</t>
-  </si>
-  <si>
-    <t>COV_Wrk</t>
   </si>
   <si>
     <t>COV_WrkPhyCon22</t>
@@ -1298,8 +1295,8 @@
   <dimension ref="A1:E1769"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A863" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E880" sqref="E880:E894"/>
+      <pane ySplit="1" topLeftCell="A1404" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1770" sqref="E1770"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3589,7 +3586,7 @@
         <v>96</v>
       </c>
       <c r="C163" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D163" t="s">
         <v>202</v>
@@ -3606,7 +3603,7 @@
         <v>96</v>
       </c>
       <c r="C164" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D164" t="s">
         <v>202</v>
@@ -3623,7 +3620,7 @@
         <v>96</v>
       </c>
       <c r="C165" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D165" t="s">
         <v>193</v>
@@ -3864,7 +3861,7 @@
         <v>106</v>
       </c>
       <c r="C182" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D182" t="s">
         <v>198</v>
@@ -3881,7 +3878,7 @@
         <v>106</v>
       </c>
       <c r="C183" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D183" t="s">
         <v>198</v>
@@ -3898,7 +3895,7 @@
         <v>106</v>
       </c>
       <c r="C184" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D184" t="s">
         <v>198</v>
@@ -3915,7 +3912,7 @@
         <v>106</v>
       </c>
       <c r="C185" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D185" t="s">
         <v>198</v>
@@ -3932,7 +3929,7 @@
         <v>106</v>
       </c>
       <c r="C186" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D186" t="s">
         <v>198</v>
@@ -3949,7 +3946,7 @@
         <v>106</v>
       </c>
       <c r="C187" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D187" t="s">
         <v>222</v>
@@ -3966,7 +3963,7 @@
         <v>106</v>
       </c>
       <c r="C188" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D188" t="s">
         <v>222</v>
@@ -3983,7 +3980,7 @@
         <v>106</v>
       </c>
       <c r="C189" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D189" t="s">
         <v>222</v>
@@ -4000,7 +3997,7 @@
         <v>106</v>
       </c>
       <c r="C190" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D190" t="s">
         <v>222</v>
@@ -4017,7 +4014,7 @@
         <v>106</v>
       </c>
       <c r="C191" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D191" t="s">
         <v>222</v>
@@ -4034,7 +4031,7 @@
         <v>106</v>
       </c>
       <c r="C192" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D192" t="s">
         <v>222</v>
@@ -4051,7 +4048,7 @@
         <v>106</v>
       </c>
       <c r="C193" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D193" t="s">
         <v>222</v>
@@ -4068,7 +4065,7 @@
         <v>106</v>
       </c>
       <c r="C194" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D194" t="s">
         <v>222</v>
@@ -4085,7 +4082,7 @@
         <v>106</v>
       </c>
       <c r="C195" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D195" t="s">
         <v>222</v>
@@ -4102,7 +4099,7 @@
         <v>106</v>
       </c>
       <c r="C196" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D196" t="s">
         <v>222</v>
@@ -4119,7 +4116,7 @@
         <v>106</v>
       </c>
       <c r="C197" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D197" t="s">
         <v>222</v>
@@ -4136,7 +4133,7 @@
         <v>106</v>
       </c>
       <c r="C198" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D198" t="s">
         <v>222</v>
@@ -4153,7 +4150,7 @@
         <v>106</v>
       </c>
       <c r="C199" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D199" t="s">
         <v>222</v>
@@ -4170,7 +4167,7 @@
         <v>106</v>
       </c>
       <c r="C200" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D200" t="s">
         <v>222</v>
@@ -4187,7 +4184,7 @@
         <v>106</v>
       </c>
       <c r="C201" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D201" t="s">
         <v>272</v>
@@ -4204,7 +4201,7 @@
         <v>106</v>
       </c>
       <c r="C202" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D202" t="s">
         <v>272</v>
@@ -4221,7 +4218,7 @@
         <v>106</v>
       </c>
       <c r="C203" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D203" t="s">
         <v>272</v>
@@ -4238,7 +4235,7 @@
         <v>106</v>
       </c>
       <c r="C204" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D204" t="s">
         <v>272</v>
@@ -4255,7 +4252,7 @@
         <v>106</v>
       </c>
       <c r="C205" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D205" t="s">
         <v>272</v>
@@ -4272,7 +4269,7 @@
         <v>106</v>
       </c>
       <c r="C206" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D206" t="s">
         <v>272</v>
@@ -4289,7 +4286,7 @@
         <v>106</v>
       </c>
       <c r="C207" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D207" t="s">
         <v>272</v>
@@ -4306,7 +4303,7 @@
         <v>106</v>
       </c>
       <c r="C208" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D208" t="s">
         <v>272</v>
@@ -4323,7 +4320,7 @@
         <v>106</v>
       </c>
       <c r="C209" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D209" t="s">
         <v>272</v>
@@ -4634,7 +4631,7 @@
         <v>49</v>
       </c>
       <c r="C231" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D231" t="s">
         <v>189</v>
@@ -4651,7 +4648,7 @@
         <v>50</v>
       </c>
       <c r="C232" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D232" t="s">
         <v>189</v>
@@ -4668,7 +4665,7 @@
         <v>50</v>
       </c>
       <c r="C233" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D233" t="s">
         <v>189</v>
@@ -4685,7 +4682,7 @@
         <v>50</v>
       </c>
       <c r="C234" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D234" t="s">
         <v>189</v>
@@ -4702,7 +4699,7 @@
         <v>50</v>
       </c>
       <c r="C235" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D235" t="s">
         <v>189</v>
@@ -4719,7 +4716,7 @@
         <v>50</v>
       </c>
       <c r="C236" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D236" t="s">
         <v>189</v>
@@ -4736,7 +4733,7 @@
         <v>50</v>
       </c>
       <c r="C237" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D237" t="s">
         <v>221</v>
@@ -6213,7 +6210,7 @@
         <v>93</v>
       </c>
       <c r="C335" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D335" t="s">
         <v>209</v>
@@ -6230,7 +6227,7 @@
         <v>93</v>
       </c>
       <c r="C336" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D336" t="s">
         <v>209</v>
@@ -6247,7 +6244,7 @@
         <v>93</v>
       </c>
       <c r="C337" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D337" t="s">
         <v>209</v>
@@ -6264,7 +6261,7 @@
         <v>93</v>
       </c>
       <c r="C338" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D338" t="s">
         <v>209</v>
@@ -6281,7 +6278,7 @@
         <v>93</v>
       </c>
       <c r="C339" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D339" t="s">
         <v>209</v>
@@ -6298,7 +6295,7 @@
         <v>93</v>
       </c>
       <c r="C340" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D340" t="s">
         <v>209</v>
@@ -6315,7 +6312,7 @@
         <v>93</v>
       </c>
       <c r="C341" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D341" t="s">
         <v>209</v>
@@ -6332,7 +6329,7 @@
         <v>93</v>
       </c>
       <c r="C342" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D342" t="s">
         <v>209</v>
@@ -6349,7 +6346,7 @@
         <v>93</v>
       </c>
       <c r="C343" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D343" t="s">
         <v>209</v>
@@ -6366,7 +6363,7 @@
         <v>93</v>
       </c>
       <c r="C344" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D344" t="s">
         <v>209</v>
@@ -7307,7 +7304,7 @@
         <v>94</v>
       </c>
       <c r="C411" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D411" t="s">
         <v>207</v>
@@ -7324,7 +7321,7 @@
         <v>94</v>
       </c>
       <c r="C412" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D412" t="s">
         <v>207</v>
@@ -7341,7 +7338,7 @@
         <v>94</v>
       </c>
       <c r="C413" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D413" t="s">
         <v>207</v>
@@ -7358,7 +7355,7 @@
         <v>94</v>
       </c>
       <c r="C414" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D414" t="s">
         <v>207</v>
@@ -7375,7 +7372,7 @@
         <v>94</v>
       </c>
       <c r="C415" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D415" t="s">
         <v>207</v>
@@ -7392,7 +7389,7 @@
         <v>94</v>
       </c>
       <c r="C416" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D416" t="s">
         <v>207</v>
@@ -7409,7 +7406,7 @@
         <v>94</v>
       </c>
       <c r="C417" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D417" t="s">
         <v>207</v>
@@ -7426,7 +7423,7 @@
         <v>94</v>
       </c>
       <c r="C418" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D418" t="s">
         <v>207</v>
@@ -7443,7 +7440,7 @@
         <v>94</v>
       </c>
       <c r="C419" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D419" t="s">
         <v>207</v>
@@ -7460,7 +7457,7 @@
         <v>94</v>
       </c>
       <c r="C420" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D420" t="s">
         <v>207</v>
@@ -7547,7 +7544,7 @@
         <v>95</v>
       </c>
       <c r="C426" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D426" t="s">
         <v>208</v>
@@ -7564,7 +7561,7 @@
         <v>95</v>
       </c>
       <c r="C427" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D427" t="s">
         <v>208</v>
@@ -7581,7 +7578,7 @@
         <v>95</v>
       </c>
       <c r="C428" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D428" t="s">
         <v>208</v>
@@ -7598,7 +7595,7 @@
         <v>95</v>
       </c>
       <c r="C429" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D429" t="s">
         <v>208</v>
@@ -7615,7 +7612,7 @@
         <v>95</v>
       </c>
       <c r="C430" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D430" t="s">
         <v>208</v>
@@ -7632,7 +7629,7 @@
         <v>95</v>
       </c>
       <c r="C431" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D431" t="s">
         <v>245</v>
@@ -7649,7 +7646,7 @@
         <v>95</v>
       </c>
       <c r="C432" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D432" t="s">
         <v>245</v>
@@ -7666,7 +7663,7 @@
         <v>95</v>
       </c>
       <c r="C433" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D433" t="s">
         <v>245</v>
@@ -7683,7 +7680,7 @@
         <v>95</v>
       </c>
       <c r="C434" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D434" t="s">
         <v>245</v>
@@ -7700,7 +7697,7 @@
         <v>95</v>
       </c>
       <c r="C435" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D435" t="s">
         <v>245</v>
@@ -8123,7 +8120,7 @@
         <v>57</v>
       </c>
       <c r="C465" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D465" t="s">
         <v>252</v>
@@ -8140,7 +8137,7 @@
         <v>57</v>
       </c>
       <c r="C466" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D466" t="s">
         <v>252</v>
@@ -8157,7 +8154,7 @@
         <v>57</v>
       </c>
       <c r="C467" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D467" t="s">
         <v>252</v>
@@ -8174,7 +8171,7 @@
         <v>57</v>
       </c>
       <c r="C468" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D468" t="s">
         <v>252</v>
@@ -8191,7 +8188,7 @@
         <v>57</v>
       </c>
       <c r="C469" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D469" t="s">
         <v>252</v>
@@ -8208,7 +8205,7 @@
         <v>57</v>
       </c>
       <c r="C470" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D470" t="s">
         <v>252</v>
@@ -8225,7 +8222,7 @@
         <v>57</v>
       </c>
       <c r="C471" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D471" t="s">
         <v>252</v>
@@ -8242,7 +8239,7 @@
         <v>57</v>
       </c>
       <c r="C472" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D472" t="s">
         <v>252</v>
@@ -8259,7 +8256,7 @@
         <v>57</v>
       </c>
       <c r="C473" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D473" t="s">
         <v>271</v>
@@ -8276,7 +8273,7 @@
         <v>57</v>
       </c>
       <c r="C474" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D474" t="s">
         <v>271</v>
@@ -8293,7 +8290,7 @@
         <v>57</v>
       </c>
       <c r="C475" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D475" t="s">
         <v>271</v>
@@ -8310,7 +8307,7 @@
         <v>57</v>
       </c>
       <c r="C476" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D476" t="s">
         <v>271</v>
@@ -8327,7 +8324,7 @@
         <v>57</v>
       </c>
       <c r="C477" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D477" t="s">
         <v>271</v>
@@ -8344,7 +8341,7 @@
         <v>57</v>
       </c>
       <c r="C478" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D478" t="s">
         <v>271</v>
@@ -9117,7 +9114,7 @@
         <v>132</v>
       </c>
       <c r="C533" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D533" t="s">
         <v>181</v>
@@ -9134,7 +9131,7 @@
         <v>133</v>
       </c>
       <c r="C534" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D534" t="s">
         <v>181</v>
@@ -9151,7 +9148,7 @@
         <v>130</v>
       </c>
       <c r="C535" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D535" t="s">
         <v>203</v>
@@ -9168,7 +9165,7 @@
         <v>130</v>
       </c>
       <c r="C536" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D536" t="s">
         <v>203</v>
@@ -9185,7 +9182,7 @@
         <v>131</v>
       </c>
       <c r="C537" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D537" t="s">
         <v>203</v>
@@ -9202,7 +9199,7 @@
         <v>131</v>
       </c>
       <c r="C538" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D538" t="s">
         <v>203</v>
@@ -9219,7 +9216,7 @@
         <v>131</v>
       </c>
       <c r="C539" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D539" t="s">
         <v>203</v>
@@ -9236,7 +9233,7 @@
         <v>131</v>
       </c>
       <c r="C540" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D540" t="s">
         <v>223</v>
@@ -9253,7 +9250,7 @@
         <v>131</v>
       </c>
       <c r="C541" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D541" t="s">
         <v>223</v>
@@ -9270,7 +9267,7 @@
         <v>131</v>
       </c>
       <c r="C542" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D542" t="s">
         <v>223</v>
@@ -9287,7 +9284,7 @@
         <v>131</v>
       </c>
       <c r="C543" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D543" t="s">
         <v>223</v>
@@ -9304,7 +9301,7 @@
         <v>131</v>
       </c>
       <c r="C544" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D544" t="s">
         <v>223</v>
@@ -9321,7 +9318,7 @@
         <v>131</v>
       </c>
       <c r="C545" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D545" t="s">
         <v>223</v>
@@ -9338,7 +9335,7 @@
         <v>131</v>
       </c>
       <c r="C546" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D546" t="s">
         <v>223</v>
@@ -9355,7 +9352,7 @@
         <v>131</v>
       </c>
       <c r="C547" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D547" t="s">
         <v>223</v>
@@ -9372,7 +9369,7 @@
         <v>131</v>
       </c>
       <c r="C548" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D548" t="s">
         <v>223</v>
@@ -9389,7 +9386,7 @@
         <v>131</v>
       </c>
       <c r="C549" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D549" t="s">
         <v>223</v>
@@ -9406,7 +9403,7 @@
         <v>131</v>
       </c>
       <c r="C550" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D550" t="s">
         <v>223</v>
@@ -9423,7 +9420,7 @@
         <v>131</v>
       </c>
       <c r="C551" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D551" t="s">
         <v>223</v>
@@ -9440,7 +9437,7 @@
         <v>131</v>
       </c>
       <c r="C552" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D552" t="s">
         <v>223</v>
@@ -9457,7 +9454,7 @@
         <v>131</v>
       </c>
       <c r="C553" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D553" t="s">
         <v>223</v>
@@ -9474,7 +9471,7 @@
         <v>131</v>
       </c>
       <c r="C554" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D554" t="s">
         <v>274</v>
@@ -9491,7 +9488,7 @@
         <v>131</v>
       </c>
       <c r="C555" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D555" t="s">
         <v>274</v>
@@ -9508,7 +9505,7 @@
         <v>131</v>
       </c>
       <c r="C556" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D556" t="s">
         <v>274</v>
@@ -9525,7 +9522,7 @@
         <v>131</v>
       </c>
       <c r="C557" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D557" t="s">
         <v>274</v>
@@ -9542,7 +9539,7 @@
         <v>131</v>
       </c>
       <c r="C558" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D558" t="s">
         <v>274</v>
@@ -9559,7 +9556,7 @@
         <v>131</v>
       </c>
       <c r="C559" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D559" t="s">
         <v>274</v>
@@ -9576,7 +9573,7 @@
         <v>131</v>
       </c>
       <c r="C560" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D560" t="s">
         <v>274</v>
@@ -9593,7 +9590,7 @@
         <v>131</v>
       </c>
       <c r="C561" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D561" t="s">
         <v>274</v>
@@ -9610,7 +9607,7 @@
         <v>131</v>
       </c>
       <c r="C562" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D562" t="s">
         <v>274</v>
@@ -9798,7 +9795,7 @@
         <v>173</v>
       </c>
       <c r="E575" t="s">
-        <v>298</v>
+        <v>62</v>
       </c>
     </row>
     <row r="576" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -9812,7 +9809,7 @@
         <v>173</v>
       </c>
       <c r="E576" t="s">
-        <v>298</v>
+        <v>62</v>
       </c>
     </row>
     <row r="577" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -9826,7 +9823,7 @@
         <v>173</v>
       </c>
       <c r="E577" t="s">
-        <v>298</v>
+        <v>62</v>
       </c>
     </row>
     <row r="578" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -11697,7 +11694,7 @@
         <v>183</v>
       </c>
       <c r="E704" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="705" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -11711,7 +11708,7 @@
         <v>183</v>
       </c>
       <c r="E705" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="706" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -12092,7 +12089,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="733" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="733" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
         <v>236</v>
       </c>
@@ -12109,7 +12106,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="734" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="734" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
         <v>246</v>
       </c>
@@ -12126,7 +12123,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="735" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="735" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
         <v>247</v>
       </c>
@@ -12143,7 +12140,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="736" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="736" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
         <v>248</v>
       </c>
@@ -12160,7 +12157,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="737" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="737" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
         <v>250</v>
       </c>
@@ -12177,7 +12174,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="738" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="738" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
         <v>253</v>
       </c>
@@ -12194,7 +12191,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="739" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="739" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
         <v>255</v>
       </c>
@@ -12211,7 +12208,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="740" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="740" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
         <v>256</v>
       </c>
@@ -12228,7 +12225,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="741" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="741" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
         <v>262</v>
       </c>
@@ -12245,7 +12242,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="742" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="742" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
         <v>263</v>
       </c>
@@ -12262,7 +12259,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="743" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="743" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A743" t="s">
         <v>264</v>
       </c>
@@ -12279,7 +12276,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="744" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="744" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
         <v>265</v>
       </c>
@@ -12296,7 +12293,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="745" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="745" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A745" t="s">
         <v>266</v>
       </c>
@@ -12313,7 +12310,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="746" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="746" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A746" t="s">
         <v>275</v>
       </c>
@@ -12330,7 +12327,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="747" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="747" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A747" t="s">
         <v>276</v>
       </c>
@@ -12347,7 +12344,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="748" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="748" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
         <v>279</v>
       </c>
@@ -12364,7 +12361,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="749" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="749" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A749" t="s">
         <v>280</v>
       </c>
@@ -12381,7 +12378,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="750" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="750" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A750" t="s">
         <v>281</v>
       </c>
@@ -12398,7 +12395,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="751" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="751" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A751" t="s">
         <v>282</v>
       </c>
@@ -12415,7 +12412,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="752" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="752" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A752" t="s">
         <v>284</v>
       </c>
@@ -12432,7 +12429,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="753" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="753" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A753" t="s">
         <v>285</v>
       </c>
@@ -12449,7 +12446,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="754" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="754" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A754" t="s">
         <v>290</v>
       </c>
@@ -12466,7 +12463,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="755" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="755" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A755" t="s">
         <v>291</v>
       </c>
@@ -12483,7 +12480,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="756" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="756" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A756" t="s">
         <v>292</v>
       </c>
@@ -12500,7 +12497,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="757" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="757" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A757" t="s">
         <v>293</v>
       </c>
@@ -12517,7 +12514,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="758" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="758" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A758" t="s">
         <v>294</v>
       </c>
@@ -12534,7 +12531,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="759" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="759" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A759" t="s">
         <v>295</v>
       </c>
@@ -12551,7 +12548,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="760" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="760" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A760" t="s">
         <v>236</v>
       </c>
@@ -12568,7 +12565,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="761" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="761" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A761" t="s">
         <v>246</v>
       </c>
@@ -12585,7 +12582,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="762" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="762" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A762" t="s">
         <v>247</v>
       </c>
@@ -12602,7 +12599,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="763" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="763" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A763" t="s">
         <v>248</v>
       </c>
@@ -12619,7 +12616,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="764" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="764" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A764" t="s">
         <v>250</v>
       </c>
@@ -12636,7 +12633,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="765" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="765" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A765" t="s">
         <v>253</v>
       </c>
@@ -12653,7 +12650,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="766" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="766" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A766" t="s">
         <v>255</v>
       </c>
@@ -12670,7 +12667,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="767" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="767" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A767" t="s">
         <v>256</v>
       </c>
@@ -12687,7 +12684,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="768" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="768" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A768" t="s">
         <v>262</v>
       </c>
@@ -12704,7 +12701,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="769" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="769" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A769" t="s">
         <v>263</v>
       </c>
@@ -12721,7 +12718,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="770" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="770" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A770" t="s">
         <v>264</v>
       </c>
@@ -12738,7 +12735,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="771" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="771" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A771" t="s">
         <v>265</v>
       </c>
@@ -12755,7 +12752,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="772" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="772" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A772" t="s">
         <v>266</v>
       </c>
@@ -12772,7 +12769,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="773" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="773" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
         <v>275</v>
       </c>
@@ -12789,7 +12786,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="774" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="774" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A774" t="s">
         <v>276</v>
       </c>
@@ -12806,7 +12803,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="775" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="775" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A775" t="s">
         <v>279</v>
       </c>
@@ -12823,7 +12820,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="776" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="776" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
         <v>280</v>
       </c>
@@ -12840,7 +12837,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="777" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="777" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A777" t="s">
         <v>281</v>
       </c>
@@ -12857,7 +12854,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="778" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="778" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A778" t="s">
         <v>282</v>
       </c>
@@ -12874,7 +12871,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="779" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="779" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A779" t="s">
         <v>284</v>
       </c>
@@ -12891,7 +12888,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="780" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="780" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A780" t="s">
         <v>285</v>
       </c>
@@ -12908,7 +12905,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="781" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="781" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A781" t="s">
         <v>290</v>
       </c>
@@ -12925,7 +12922,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="782" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="782" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A782" t="s">
         <v>291</v>
       </c>
@@ -12942,7 +12939,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="783" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="783" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A783" t="s">
         <v>292</v>
       </c>
@@ -12959,7 +12956,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="784" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="784" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A784" t="s">
         <v>293</v>
       </c>
@@ -12976,7 +12973,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="785" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="785" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A785" t="s">
         <v>294</v>
       </c>
@@ -12993,7 +12990,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="786" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="786" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A786" t="s">
         <v>295</v>
       </c>
@@ -13010,7 +13007,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="787" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="787" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A787" t="s">
         <v>236</v>
       </c>
@@ -13027,7 +13024,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="788" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="788" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A788" t="s">
         <v>246</v>
       </c>
@@ -13044,7 +13041,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="789" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="789" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A789" t="s">
         <v>247</v>
       </c>
@@ -13061,7 +13058,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="790" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="790" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A790" t="s">
         <v>248</v>
       </c>
@@ -13078,7 +13075,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="791" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="791" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A791" t="s">
         <v>250</v>
       </c>
@@ -13095,7 +13092,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="792" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="792" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A792" t="s">
         <v>253</v>
       </c>
@@ -13112,7 +13109,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="793" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="793" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A793" t="s">
         <v>255</v>
       </c>
@@ -13129,7 +13126,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="794" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="794" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A794" t="s">
         <v>256</v>
       </c>
@@ -13146,7 +13143,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="795" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="795" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A795" t="s">
         <v>262</v>
       </c>
@@ -13163,7 +13160,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="796" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="796" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A796" t="s">
         <v>263</v>
       </c>
@@ -13180,7 +13177,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="797" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="797" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A797" t="s">
         <v>264</v>
       </c>
@@ -13197,7 +13194,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="798" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="798" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A798" t="s">
         <v>265</v>
       </c>
@@ -13214,7 +13211,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="799" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="799" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A799" t="s">
         <v>266</v>
       </c>
@@ -13231,7 +13228,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="800" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="800" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A800" t="s">
         <v>275</v>
       </c>
@@ -13248,7 +13245,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="801" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="801" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A801" t="s">
         <v>276</v>
       </c>
@@ -13265,7 +13262,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="802" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="802" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A802" t="s">
         <v>279</v>
       </c>
@@ -13282,7 +13279,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="803" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="803" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A803" t="s">
         <v>280</v>
       </c>
@@ -13299,7 +13296,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="804" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="804" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A804" t="s">
         <v>281</v>
       </c>
@@ -13316,7 +13313,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="805" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="805" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A805" t="s">
         <v>282</v>
       </c>
@@ -13333,7 +13330,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="806" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="806" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A806" t="s">
         <v>284</v>
       </c>
@@ -13350,7 +13347,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="807" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="807" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A807" t="s">
         <v>285</v>
       </c>
@@ -13367,7 +13364,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="808" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="808" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A808" t="s">
         <v>290</v>
       </c>
@@ -13384,7 +13381,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="809" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="809" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A809" t="s">
         <v>291</v>
       </c>
@@ -13401,7 +13398,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="810" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="810" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A810" t="s">
         <v>292</v>
       </c>
@@ -13418,7 +13415,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="811" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="811" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A811" t="s">
         <v>293</v>
       </c>
@@ -13435,7 +13432,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="812" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="812" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A812" t="s">
         <v>294</v>
       </c>
@@ -13452,7 +13449,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="813" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="813" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A813" t="s">
         <v>295</v>
       </c>
@@ -13469,7 +13466,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="814" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="814" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A814" t="s">
         <v>236</v>
       </c>
@@ -13486,7 +13483,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="815" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="815" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A815" t="s">
         <v>246</v>
       </c>
@@ -13503,7 +13500,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="816" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="816" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A816" t="s">
         <v>247</v>
       </c>
@@ -13520,7 +13517,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="817" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="817" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A817" t="s">
         <v>248</v>
       </c>
@@ -13537,7 +13534,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="818" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="818" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A818" t="s">
         <v>250</v>
       </c>
@@ -13554,7 +13551,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="819" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="819" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A819" t="s">
         <v>253</v>
       </c>
@@ -13571,7 +13568,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="820" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="820" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A820" t="s">
         <v>255</v>
       </c>
@@ -13588,7 +13585,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="821" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="821" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A821" t="s">
         <v>256</v>
       </c>
@@ -13605,7 +13602,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="822" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="822" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A822" t="s">
         <v>262</v>
       </c>
@@ -13622,7 +13619,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="823" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="823" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A823" t="s">
         <v>263</v>
       </c>
@@ -13639,7 +13636,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="824" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="824" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A824" t="s">
         <v>264</v>
       </c>
@@ -13656,7 +13653,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="825" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="825" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A825" t="s">
         <v>265</v>
       </c>
@@ -13673,7 +13670,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="826" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="826" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A826" t="s">
         <v>266</v>
       </c>
@@ -13690,7 +13687,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="827" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="827" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A827" t="s">
         <v>275</v>
       </c>
@@ -13707,7 +13704,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="828" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="828" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A828" t="s">
         <v>276</v>
       </c>
@@ -13724,7 +13721,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="829" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="829" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A829" t="s">
         <v>279</v>
       </c>
@@ -13741,7 +13738,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="830" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="830" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A830" t="s">
         <v>280</v>
       </c>
@@ -13758,7 +13755,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="831" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="831" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A831" t="s">
         <v>281</v>
       </c>
@@ -13775,7 +13772,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="832" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="832" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A832" t="s">
         <v>282</v>
       </c>
@@ -13792,7 +13789,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="833" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="833" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A833" t="s">
         <v>284</v>
       </c>
@@ -13809,7 +13806,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="834" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="834" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A834" t="s">
         <v>285</v>
       </c>
@@ -13826,7 +13823,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="835" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="835" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A835" t="s">
         <v>290</v>
       </c>
@@ -13843,7 +13840,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="836" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="836" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A836" t="s">
         <v>291</v>
       </c>
@@ -13860,7 +13857,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="837" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="837" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A837" t="s">
         <v>292</v>
       </c>
@@ -13877,7 +13874,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="838" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="838" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A838" t="s">
         <v>293</v>
       </c>
@@ -13894,7 +13891,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="839" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="839" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A839" t="s">
         <v>294</v>
       </c>
@@ -13911,7 +13908,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="840" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="840" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A840" t="s">
         <v>295</v>
       </c>
@@ -13928,7 +13925,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="841" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="841" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A841" t="s">
         <v>236</v>
       </c>
@@ -13945,7 +13942,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="842" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="842" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A842" t="s">
         <v>246</v>
       </c>
@@ -13962,7 +13959,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="843" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="843" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A843" t="s">
         <v>247</v>
       </c>
@@ -13979,7 +13976,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="844" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="844" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A844" t="s">
         <v>248</v>
       </c>
@@ -13996,7 +13993,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="845" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="845" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A845" t="s">
         <v>250</v>
       </c>
@@ -14013,7 +14010,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="846" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="846" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A846" t="s">
         <v>253</v>
       </c>
@@ -14030,7 +14027,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="847" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="847" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A847" t="s">
         <v>255</v>
       </c>
@@ -14047,7 +14044,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="848" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="848" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A848" t="s">
         <v>256</v>
       </c>
@@ -14064,7 +14061,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="849" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="849" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A849" t="s">
         <v>262</v>
       </c>
@@ -14081,7 +14078,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="850" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="850" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A850" t="s">
         <v>263</v>
       </c>
@@ -14098,7 +14095,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="851" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="851" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A851" t="s">
         <v>264</v>
       </c>
@@ -14115,7 +14112,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="852" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="852" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A852" t="s">
         <v>265</v>
       </c>
@@ -14132,7 +14129,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="853" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="853" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A853" t="s">
         <v>266</v>
       </c>
@@ -14149,7 +14146,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="854" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="854" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A854" t="s">
         <v>275</v>
       </c>
@@ -14166,7 +14163,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="855" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="855" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A855" t="s">
         <v>276</v>
       </c>
@@ -14183,7 +14180,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="856" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="856" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A856" t="s">
         <v>279</v>
       </c>
@@ -14200,7 +14197,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="857" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="857" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A857" t="s">
         <v>280</v>
       </c>
@@ -14217,7 +14214,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="858" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="858" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A858" t="s">
         <v>281</v>
       </c>
@@ -14234,7 +14231,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="859" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="859" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A859" t="s">
         <v>282</v>
       </c>
@@ -14251,7 +14248,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="860" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="860" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A860" t="s">
         <v>284</v>
       </c>
@@ -14268,7 +14265,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="861" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="861" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A861" t="s">
         <v>285</v>
       </c>
@@ -14285,7 +14282,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="862" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="862" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A862" t="s">
         <v>290</v>
       </c>
@@ -14302,7 +14299,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="863" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="863" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A863" t="s">
         <v>291</v>
       </c>
@@ -14319,7 +14316,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="864" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="864" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A864" t="s">
         <v>292</v>
       </c>
@@ -14336,7 +14333,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="865" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="865" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A865" t="s">
         <v>293</v>
       </c>
@@ -14353,7 +14350,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="866" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="866" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A866" t="s">
         <v>294</v>
       </c>
@@ -14370,7 +14367,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="867" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="867" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A867" t="s">
         <v>295</v>
       </c>
@@ -14387,7 +14384,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="868" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="868" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A868" t="s">
         <v>236</v>
       </c>
@@ -14401,7 +14398,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="869" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="869" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A869" t="s">
         <v>246</v>
       </c>
@@ -14415,7 +14412,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="870" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="870" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A870" t="s">
         <v>247</v>
       </c>
@@ -14429,7 +14426,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="871" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="871" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A871" t="s">
         <v>248</v>
       </c>
@@ -14443,7 +14440,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="872" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="872" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A872" t="s">
         <v>250</v>
       </c>
@@ -14457,7 +14454,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="873" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="873" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A873" t="s">
         <v>253</v>
       </c>
@@ -14471,7 +14468,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="874" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="874" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A874" t="s">
         <v>255</v>
       </c>
@@ -14485,7 +14482,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="875" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="875" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A875" t="s">
         <v>256</v>
       </c>
@@ -14499,7 +14496,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="876" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="876" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A876" t="s">
         <v>262</v>
       </c>
@@ -14513,7 +14510,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="877" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="877" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A877" t="s">
         <v>263</v>
       </c>
@@ -14527,7 +14524,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="878" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="878" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A878" t="s">
         <v>264</v>
       </c>
@@ -14541,7 +14538,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="879" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="879" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A879" t="s">
         <v>265</v>
       </c>
@@ -14555,7 +14552,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="880" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="880" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A880" t="s">
         <v>266</v>
       </c>
@@ -14569,7 +14566,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="881" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="881" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A881" t="s">
         <v>275</v>
       </c>
@@ -14583,7 +14580,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="882" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="882" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A882" t="s">
         <v>276</v>
       </c>
@@ -14597,7 +14594,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="883" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="883" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A883" t="s">
         <v>279</v>
       </c>
@@ -14611,7 +14608,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="884" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="884" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A884" t="s">
         <v>280</v>
       </c>
@@ -14625,7 +14622,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="885" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="885" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A885" t="s">
         <v>281</v>
       </c>
@@ -14639,7 +14636,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="886" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="886" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A886" t="s">
         <v>282</v>
       </c>
@@ -14653,7 +14650,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="887" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="887" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A887" t="s">
         <v>284</v>
       </c>
@@ -14667,7 +14664,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="888" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="888" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A888" t="s">
         <v>285</v>
       </c>
@@ -14681,7 +14678,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="889" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="889" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A889" t="s">
         <v>290</v>
       </c>
@@ -14695,7 +14692,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="890" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="890" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A890" t="s">
         <v>291</v>
       </c>
@@ -14709,7 +14706,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="891" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="891" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A891" t="s">
         <v>292</v>
       </c>
@@ -14723,7 +14720,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="892" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="892" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A892" t="s">
         <v>293</v>
       </c>
@@ -14737,7 +14734,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="893" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="893" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A893" t="s">
         <v>294</v>
       </c>
@@ -14751,7 +14748,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="894" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="894" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A894" t="s">
         <v>295</v>
       </c>
@@ -14765,7 +14762,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="895" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="895" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A895" t="s">
         <v>236</v>
       </c>
@@ -14773,7 +14770,7 @@
         <v>41</v>
       </c>
       <c r="C895" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D895" t="s">
         <v>238</v>
@@ -14782,7 +14779,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="896" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="896" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A896" t="s">
         <v>246</v>
       </c>
@@ -14790,7 +14787,7 @@
         <v>41</v>
       </c>
       <c r="C896" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D896" t="s">
         <v>238</v>
@@ -14799,7 +14796,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="897" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="897" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A897" t="s">
         <v>247</v>
       </c>
@@ -14807,7 +14804,7 @@
         <v>41</v>
       </c>
       <c r="C897" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D897" t="s">
         <v>238</v>
@@ -14816,7 +14813,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="898" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="898" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A898" t="s">
         <v>248</v>
       </c>
@@ -14824,7 +14821,7 @@
         <v>41</v>
       </c>
       <c r="C898" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D898" t="s">
         <v>238</v>
@@ -14833,7 +14830,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="899" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="899" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A899" t="s">
         <v>250</v>
       </c>
@@ -14841,7 +14838,7 @@
         <v>41</v>
       </c>
       <c r="C899" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D899" t="s">
         <v>238</v>
@@ -14850,7 +14847,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="900" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="900" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A900" t="s">
         <v>253</v>
       </c>
@@ -14858,7 +14855,7 @@
         <v>41</v>
       </c>
       <c r="C900" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D900" t="s">
         <v>238</v>
@@ -14867,7 +14864,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="901" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="901" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A901" t="s">
         <v>255</v>
       </c>
@@ -14875,7 +14872,7 @@
         <v>41</v>
       </c>
       <c r="C901" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D901" t="s">
         <v>238</v>
@@ -14884,7 +14881,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="902" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="902" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A902" t="s">
         <v>256</v>
       </c>
@@ -14892,7 +14889,7 @@
         <v>41</v>
       </c>
       <c r="C902" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D902" t="s">
         <v>238</v>
@@ -14901,7 +14898,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="903" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="903" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A903" t="s">
         <v>262</v>
       </c>
@@ -14909,7 +14906,7 @@
         <v>41</v>
       </c>
       <c r="C903" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D903" t="s">
         <v>238</v>
@@ -14918,7 +14915,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="904" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="904" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A904" t="s">
         <v>263</v>
       </c>
@@ -14926,7 +14923,7 @@
         <v>41</v>
       </c>
       <c r="C904" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D904" t="s">
         <v>238</v>
@@ -14935,7 +14932,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="905" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="905" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A905" t="s">
         <v>264</v>
       </c>
@@ -14943,7 +14940,7 @@
         <v>41</v>
       </c>
       <c r="C905" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D905" t="s">
         <v>238</v>
@@ -14952,7 +14949,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="906" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="906" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A906" t="s">
         <v>265</v>
       </c>
@@ -14960,7 +14957,7 @@
         <v>41</v>
       </c>
       <c r="C906" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D906" t="s">
         <v>238</v>
@@ -14969,7 +14966,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="907" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="907" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A907" t="s">
         <v>266</v>
       </c>
@@ -14977,7 +14974,7 @@
         <v>41</v>
       </c>
       <c r="C907" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D907" t="s">
         <v>238</v>
@@ -14986,7 +14983,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="908" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="908" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A908" t="s">
         <v>275</v>
       </c>
@@ -14994,7 +14991,7 @@
         <v>41</v>
       </c>
       <c r="C908" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D908" t="s">
         <v>238</v>
@@ -15003,7 +15000,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="909" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="909" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A909" t="s">
         <v>276</v>
       </c>
@@ -15011,7 +15008,7 @@
         <v>41</v>
       </c>
       <c r="C909" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D909" t="s">
         <v>238</v>
@@ -15020,7 +15017,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="910" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="910" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A910" t="s">
         <v>279</v>
       </c>
@@ -15028,7 +15025,7 @@
         <v>41</v>
       </c>
       <c r="C910" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D910" t="s">
         <v>238</v>
@@ -15037,7 +15034,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="911" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="911" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A911" t="s">
         <v>280</v>
       </c>
@@ -15045,7 +15042,7 @@
         <v>41</v>
       </c>
       <c r="C911" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D911" t="s">
         <v>238</v>
@@ -15054,7 +15051,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="912" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="912" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A912" t="s">
         <v>281</v>
       </c>
@@ -15062,7 +15059,7 @@
         <v>41</v>
       </c>
       <c r="C912" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D912" t="s">
         <v>238</v>
@@ -15071,7 +15068,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="913" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="913" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A913" t="s">
         <v>282</v>
       </c>
@@ -15079,7 +15076,7 @@
         <v>41</v>
       </c>
       <c r="C913" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D913" t="s">
         <v>238</v>
@@ -15088,7 +15085,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="914" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="914" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A914" t="s">
         <v>284</v>
       </c>
@@ -15096,7 +15093,7 @@
         <v>41</v>
       </c>
       <c r="C914" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D914" t="s">
         <v>238</v>
@@ -15105,7 +15102,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="915" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="915" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A915" t="s">
         <v>285</v>
       </c>
@@ -15113,7 +15110,7 @@
         <v>41</v>
       </c>
       <c r="C915" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D915" t="s">
         <v>238</v>
@@ -15130,7 +15127,7 @@
         <v>54</v>
       </c>
       <c r="C916" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D916" t="s">
         <v>176</v>
@@ -15147,7 +15144,7 @@
         <v>55</v>
       </c>
       <c r="C917" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D917" t="s">
         <v>176</v>
@@ -15164,7 +15161,7 @@
         <v>56</v>
       </c>
       <c r="C918" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D918" t="s">
         <v>176</v>
@@ -15181,7 +15178,7 @@
         <v>56</v>
       </c>
       <c r="C919" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D919" t="s">
         <v>176</v>
@@ -15198,7 +15195,7 @@
         <v>56</v>
       </c>
       <c r="C920" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D920" t="s">
         <v>176</v>
@@ -15215,7 +15212,7 @@
         <v>56</v>
       </c>
       <c r="C921" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D921" t="s">
         <v>176</v>
@@ -15232,7 +15229,7 @@
         <v>56</v>
       </c>
       <c r="C922" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D922" t="s">
         <v>176</v>
@@ -15249,7 +15246,7 @@
         <v>56</v>
       </c>
       <c r="C923" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D923" t="s">
         <v>219</v>
@@ -15266,7 +15263,7 @@
         <v>56</v>
       </c>
       <c r="C924" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D924" t="s">
         <v>219</v>
@@ -15283,7 +15280,7 @@
         <v>56</v>
       </c>
       <c r="C925" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D925" t="s">
         <v>219</v>
@@ -15300,7 +15297,7 @@
         <v>56</v>
       </c>
       <c r="C926" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D926" t="s">
         <v>219</v>
@@ -15317,7 +15314,7 @@
         <v>56</v>
       </c>
       <c r="C927" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D927" t="s">
         <v>219</v>
@@ -15334,7 +15331,7 @@
         <v>56</v>
       </c>
       <c r="C928" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D928" t="s">
         <v>219</v>
@@ -15351,7 +15348,7 @@
         <v>56</v>
       </c>
       <c r="C929" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D929" t="s">
         <v>219</v>
@@ -15368,7 +15365,7 @@
         <v>56</v>
       </c>
       <c r="C930" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D930" t="s">
         <v>219</v>
@@ -15385,7 +15382,7 @@
         <v>56</v>
       </c>
       <c r="C931" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D931" t="s">
         <v>219</v>
@@ -15402,7 +15399,7 @@
         <v>56</v>
       </c>
       <c r="C932" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D932" t="s">
         <v>219</v>
@@ -15419,7 +15416,7 @@
         <v>56</v>
       </c>
       <c r="C933" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D933" t="s">
         <v>219</v>
@@ -15436,7 +15433,7 @@
         <v>56</v>
       </c>
       <c r="C934" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D934" t="s">
         <v>219</v>
@@ -15453,7 +15450,7 @@
         <v>56</v>
       </c>
       <c r="C935" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D935" t="s">
         <v>219</v>
@@ -15470,7 +15467,7 @@
         <v>56</v>
       </c>
       <c r="C936" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D936" t="s">
         <v>219</v>
@@ -15487,7 +15484,7 @@
         <v>56</v>
       </c>
       <c r="C937" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D937" t="s">
         <v>269</v>
@@ -15504,7 +15501,7 @@
         <v>56</v>
       </c>
       <c r="C938" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D938" t="s">
         <v>269</v>
@@ -15521,7 +15518,7 @@
         <v>56</v>
       </c>
       <c r="C939" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D939" t="s">
         <v>269</v>
@@ -15538,7 +15535,7 @@
         <v>56</v>
       </c>
       <c r="C940" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D940" t="s">
         <v>269</v>
@@ -15555,7 +15552,7 @@
         <v>56</v>
       </c>
       <c r="C941" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D941" t="s">
         <v>269</v>
@@ -15572,7 +15569,7 @@
         <v>56</v>
       </c>
       <c r="C942" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D942" t="s">
         <v>269</v>
@@ -15589,7 +15586,7 @@
         <v>56</v>
       </c>
       <c r="C943" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D943" t="s">
         <v>269</v>
@@ -15606,7 +15603,7 @@
         <v>56</v>
       </c>
       <c r="C944" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D944" t="s">
         <v>269</v>
@@ -15623,7 +15620,7 @@
         <v>56</v>
       </c>
       <c r="C945" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D945" t="s">
         <v>269</v>
@@ -21638,7 +21635,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="1375" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1375" t="s">
         <v>137</v>
       </c>
@@ -21652,7 +21649,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1376" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1376" t="s">
         <v>165</v>
       </c>
@@ -21666,7 +21663,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1377" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1377" t="s">
         <v>167</v>
       </c>
@@ -21680,7 +21677,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1378" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1378" t="s">
         <v>174</v>
       </c>
@@ -21694,7 +21691,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1379" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1379" t="s">
         <v>187</v>
       </c>
@@ -21708,7 +21705,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1380" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1380" t="s">
         <v>197</v>
       </c>
@@ -21722,7 +21719,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1381" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1381" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1381" t="s">
         <v>204</v>
       </c>
@@ -21736,7 +21733,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1382" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1382" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1382" t="s">
         <v>205</v>
       </c>
@@ -21750,7 +21747,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1383" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1383" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1383" t="s">
         <v>211</v>
       </c>
@@ -21764,7 +21761,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1384" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1384" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1384" t="s">
         <v>215</v>
       </c>
@@ -21778,7 +21775,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1385" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1385" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1385" t="s">
         <v>216</v>
       </c>
@@ -21792,7 +21789,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1386" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1386" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1386" t="s">
         <v>224</v>
       </c>
@@ -21806,7 +21803,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1387" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1387" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1387" t="s">
         <v>236</v>
       </c>
@@ -21820,7 +21817,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1388" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1388" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1388" t="s">
         <v>246</v>
       </c>
@@ -21834,7 +21831,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1389" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1389" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1389" t="s">
         <v>247</v>
       </c>
@@ -21848,7 +21845,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1390" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1390" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1390" t="s">
         <v>248</v>
       </c>
@@ -21862,7 +21859,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1391" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1391" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1391" t="s">
         <v>250</v>
       </c>
@@ -21876,7 +21873,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1392" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1392" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1392" t="s">
         <v>253</v>
       </c>
@@ -21890,7 +21887,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1393" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1393" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1393" t="s">
         <v>255</v>
       </c>
@@ -21904,7 +21901,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1394" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1394" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1394" t="s">
         <v>256</v>
       </c>
@@ -21918,7 +21915,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1395" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1395" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1395" t="s">
         <v>262</v>
       </c>
@@ -21932,7 +21929,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1396" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1396" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1396" t="s">
         <v>263</v>
       </c>
@@ -21946,7 +21943,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1397" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1397" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1397" t="s">
         <v>264</v>
       </c>
@@ -21960,7 +21957,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1398" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1398" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1398" t="s">
         <v>265</v>
       </c>
@@ -21974,7 +21971,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1399" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1399" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1399" t="s">
         <v>266</v>
       </c>
@@ -21988,7 +21985,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1400" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1400" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1400" t="s">
         <v>275</v>
       </c>
@@ -22002,7 +21999,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1401" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1401" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1401" t="s">
         <v>276</v>
       </c>
@@ -22016,7 +22013,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1402" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1402" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1402" t="s">
         <v>279</v>
       </c>
@@ -22030,7 +22027,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1403" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1403" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1403" t="s">
         <v>280</v>
       </c>
@@ -22044,7 +22041,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1404" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1404" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1404" t="s">
         <v>281</v>
       </c>
@@ -22058,7 +22055,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1405" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1405" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1405" t="s">
         <v>282</v>
       </c>
@@ -22072,7 +22069,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1406" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1406" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1406" t="s">
         <v>284</v>
       </c>
@@ -22086,7 +22083,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1407" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1407" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1407" t="s">
         <v>290</v>
       </c>
@@ -22100,7 +22097,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1408" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1408" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1408" t="s">
         <v>291</v>
       </c>
@@ -22114,7 +22111,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1409" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1409" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1409" t="s">
         <v>292</v>
       </c>
@@ -22128,7 +22125,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1410" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1410" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1410" t="s">
         <v>293</v>
       </c>
@@ -22142,7 +22139,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1411" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1411" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1411" t="s">
         <v>294</v>
       </c>
@@ -22156,7 +22153,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1412" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1412" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1412" t="s">
         <v>295</v>
       </c>
@@ -22170,7 +22167,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1413" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1413" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1413" t="s">
         <v>285</v>
       </c>
@@ -22184,15 +22181,15 @@
         <v>147</v>
       </c>
     </row>
-    <row r="1414" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1414" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1414" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D1414" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E1414" t="s">
-        <v>147</v>
+        <v>304</v>
       </c>
     </row>
     <row r="1415" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -24381,13 +24378,13 @@
     </row>
     <row r="1571" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B1571" t="s">
+        <v>307</v>
+      </c>
+      <c r="D1571" t="s">
         <v>308</v>
       </c>
-      <c r="D1571" t="s">
-        <v>309</v>
-      </c>
       <c r="E1571" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="1572" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -25484,13 +25481,13 @@
     </row>
     <row r="1650" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B1650" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D1650" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E1650" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="1651" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -26587,13 +26584,13 @@
     </row>
     <row r="1729" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B1729" t="s">
+        <v>302</v>
+      </c>
+      <c r="D1729" t="s">
         <v>303</v>
       </c>
-      <c r="D1729" t="s">
-        <v>304</v>
-      </c>
       <c r="E1729" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="1730" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -27144,38 +27141,43 @@
     </row>
     <row r="1769" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B1769" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D1769" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E1769" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1769">
-    <filterColumn colId="4">
+    <filterColumn colId="1">
       <filters>
-        <filter val="COV_WrkRea_emplwrkhom"/>
-        <filter val="COV_WrkRea_govadvice"/>
-        <filter val="COV_WrkRea_nochildcare"/>
-        <filter val="COV_WrkRea_normhome"/>
-        <filter val="COV_WrkRea_wrkclose"/>
-        <filter val="COV_WrkRea01"/>
-        <filter val="COV_WrkReaB01"/>
-        <filter val="COV_WrkReaSp"/>
+        <filter val="Month"/>
       </filters>
     </filterColumn>
-    <sortState ref="A733:E915">
-      <sortCondition ref="E1:E1769"/>
-    </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008705DFD2773E994AB5E781DE9A247DE5" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dbb928eeaae5bb703b8dc14306bc3608">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="875267d4-4f4f-46a7-b55f-6d43fcf74f9f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="aca4360c3200e37316c4f7918bfc6b7b" ns3:_="">
     <xsd:import namespace="875267d4-4f4f-46a7-b55f-6d43fcf74f9f"/>
@@ -27353,22 +27355,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3D8607E-996C-45D3-AB87-93D06FEA0777}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="875267d4-4f4f-46a7-b55f-6d43fcf74f9f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CAE885B-162A-4480-B332-62748824F5FF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{454D0352-3722-4DF6-A396-2093DD676256}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27384,28 +27395,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CAE885B-162A-4480-B332-62748824F5FF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3D8607E-996C-45D3-AB87-93D06FEA0777}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="875267d4-4f4f-46a7-b55f-6d43fcf74f9f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>